<commit_message>
Added Burndown chart.xlsx and Sprint Backlog.xlsx for Sprint 1
</commit_message>
<xml_diff>
--- a/Project/Phase 1/Sprint 1/Burndown chart.xlsx
+++ b/Project/Phase 1/Sprint 1/Burndown chart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="EsteLivro" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sophia\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sophia\Desktop\Sophia\Faculdade\ES\GanttProject\Project\Phase 1\Sprint 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4756362-1DC1-458F-91AA-C23C3D24641A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2EB2B46-1641-4DEF-A0E9-3D756D5D596E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Sprint Burndown Chart</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>Ideal Burndown</t>
-  </si>
-  <si>
-    <t>Identify three GoF design patterns.</t>
   </si>
 </sst>
 </file>
@@ -162,7 +159,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -407,37 +404,11 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -447,9 +418,46 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -460,9 +468,7 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -472,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -480,9 +486,6 @@
     <xf numFmtId="165" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -519,12 +522,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -539,16 +536,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -558,7 +549,10 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -573,18 +567,6 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -603,21 +585,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -722,7 +739,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Burndown Chart'!$B$11:$C$11</c:f>
+              <c:f>'Burndown Chart'!$B$21:$C$21</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -743,7 +760,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$D$11:$G$11</c:f>
+              <c:f>'Burndown Chart'!$D$21:$G$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -754,10 +771,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -789,7 +806,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Burndown Chart'!$B$12:$C$12</c:f>
+              <c:f>'Burndown Chart'!$B$22:$C$22</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -844,21 +861,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$D$12:$G$12</c:f>
+              <c:f>'Burndown Chart'!$D$22:$G$22</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>10</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -875,7 +892,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Burndown Chart'!$B$13:$C$13</c:f>
+              <c:f>'Burndown Chart'!$B$23:$C$23</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -918,18 +935,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$D$13:$G$13</c:f>
+              <c:f>'Burndown Chart'!$D$23:$G$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>10</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.6666666666666661</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.333333333333333</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1012,7 +1029,7 @@
         <c:axId val="1048433599"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="11"/>
+          <c:max val="31"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1120,6 +1137,7 @@
         <c:crossAx val="1048432767"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1766,13 +1784,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>7842</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>108697</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>681317</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>105336</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2101,10 +2119,10 @@
   <sheetPr codeName="Folha1">
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="B1:H13"/>
+  <dimension ref="B1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2115,206 +2133,400 @@
     <col min="5" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:8" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="38" t="s">
+    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:7" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="40"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="32"/>
     </row>
-    <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="41"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="43"/>
+    <row r="3" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="33"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="35"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="32" t="s">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="C4" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>44851</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>44852</v>
       </c>
-      <c r="G4" s="47">
+      <c r="G4" s="24">
         <v>44853</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="33"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="6" t="s">
+    <row r="5" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="29"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="23">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="50">
         <v>1</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="20" t="str">
+        <f>"Identify #"&amp;B6&amp;" GoF design pattern"</f>
+        <v>Identify #1 GoF design pattern</v>
+      </c>
+      <c r="D6" s="22">
+        <v>2</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="8">
+        <v>1</v>
+      </c>
+      <c r="G6" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="51">
+        <v>2</v>
+      </c>
+      <c r="C7" s="21" t="str">
+        <f t="shared" ref="C7:C20" si="0">"Identify #"&amp;B7&amp;" GoF design pattern"</f>
+        <v>Identify #2 GoF design pattern</v>
+      </c>
+      <c r="D7" s="23">
+        <v>2</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="11">
+        <v>1</v>
+      </c>
+      <c r="G7" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="51">
+        <v>3</v>
+      </c>
+      <c r="C8" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>Identify #3 GoF design pattern</v>
+      </c>
+      <c r="D8" s="23">
+        <v>2</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="11">
+        <v>1</v>
+      </c>
+      <c r="G8" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="51">
+        <v>4</v>
+      </c>
+      <c r="C9" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>Identify #4 GoF design pattern</v>
+      </c>
+      <c r="D9" s="23">
+        <v>2</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="51">
+        <v>5</v>
+      </c>
+      <c r="C10" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>Identify #5 GoF design pattern</v>
+      </c>
+      <c r="D10" s="23">
+        <v>2</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="51">
+        <v>6</v>
+      </c>
+      <c r="C11" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>Identify #6 GoF design pattern</v>
+      </c>
+      <c r="D11" s="23">
+        <v>2</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="51">
+        <v>7</v>
+      </c>
+      <c r="C12" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>Identify #7 GoF design pattern</v>
+      </c>
+      <c r="D12" s="23">
+        <v>2</v>
+      </c>
+      <c r="E12" s="14"/>
+      <c r="F12" s="11">
+        <v>1</v>
+      </c>
+      <c r="G12" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="51">
+        <v>8</v>
+      </c>
+      <c r="C13" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>Identify #8 GoF design pattern</v>
+      </c>
+      <c r="D13" s="23">
+        <v>2</v>
+      </c>
+      <c r="E13" s="14"/>
+      <c r="F13" s="11">
+        <v>1</v>
+      </c>
+      <c r="G13" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="51">
+        <v>9</v>
+      </c>
+      <c r="C14" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>Identify #9 GoF design pattern</v>
+      </c>
+      <c r="D14" s="23">
+        <v>2</v>
+      </c>
+      <c r="E14" s="14"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="51">
+        <v>10</v>
+      </c>
+      <c r="C15" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>Identify #10 GoF design pattern</v>
+      </c>
+      <c r="D15" s="23">
+        <v>2</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="51">
         <v>11</v>
       </c>
-      <c r="D6" s="27">
-        <v>2</v>
-      </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="10"/>
+      <c r="C16" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>Identify #11 GoF design pattern</v>
+      </c>
+      <c r="D16" s="23">
+        <v>2</v>
+      </c>
+      <c r="E16" s="14"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="12">
+        <v>2</v>
+      </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="25">
-        <v>2</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="28">
-        <v>2</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="13"/>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="51">
+        <v>12</v>
+      </c>
+      <c r="C17" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>Identify #12 GoF design pattern</v>
+      </c>
+      <c r="D17" s="23">
+        <v>2</v>
+      </c>
+      <c r="E17" s="14"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="12">
+        <v>2</v>
+      </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="25">
-        <v>3</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="28">
-        <v>2</v>
-      </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="13"/>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="51">
+        <v>13</v>
+      </c>
+      <c r="C18" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>Identify #13 GoF design pattern</v>
+      </c>
+      <c r="D18" s="23">
+        <v>2</v>
+      </c>
+      <c r="E18" s="14"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="12">
+        <v>2</v>
+      </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="25">
-        <v>4</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="28">
-        <v>2</v>
-      </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="13"/>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="51">
+        <v>14</v>
+      </c>
+      <c r="C19" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>Identify #14 GoF design pattern</v>
+      </c>
+      <c r="D19" s="23">
+        <v>2</v>
+      </c>
+      <c r="E19" s="14"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="12">
+        <v>2</v>
+      </c>
     </row>
-    <row r="10" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="25">
+    <row r="20" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="52">
+        <v>15</v>
+      </c>
+      <c r="C20" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>Identify #15 GoF design pattern</v>
+      </c>
+      <c r="D20" s="46">
+        <v>2</v>
+      </c>
+      <c r="E20" s="47"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="40"/>
+      <c r="D21" s="42">
+        <v>0</v>
+      </c>
+      <c r="E21" s="43">
+        <f>SUM(E6:E20)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="43">
+        <f>SUM(F6:F20)</f>
         <v>5</v>
       </c>
-      <c r="C10" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="29">
-        <v>2</v>
-      </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="13"/>
+      <c r="G21" s="44">
+        <f>SUM(G6:G20)</f>
+        <v>25</v>
+      </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="45"/>
-      <c r="D11" s="3">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="39"/>
+      <c r="D22" s="16">
+        <f>SUM(D6:D21)</f>
+        <v>30</v>
+      </c>
+      <c r="E22" s="17">
+        <f>D22-SUM(E6:E20)</f>
+        <v>30</v>
+      </c>
+      <c r="F22" s="15">
+        <f>E22-SUM(F6:F20)</f>
+        <v>25</v>
+      </c>
+      <c r="G22" s="25">
+        <f>F22-SUM(G6:G20)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="17">
-        <f>SUM(E6:E10)</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="17">
-        <f>SUM(F6:F10)</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="48">
-        <f>SUM(G6:G10)</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="46"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="35"/>
-      <c r="D12" s="19">
-        <f>SUM(D6:D11)</f>
+    <row r="23" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="20">
-        <f>D12-SUM(E6:E10)</f>
+      <c r="C23" s="37"/>
+      <c r="D23" s="18">
+        <f>D22</f>
+        <v>30</v>
+      </c>
+      <c r="E23" s="19">
+        <f>$D$23-($D$23/(COLUMNS(E5:G5))*COLUMNS(E5))</f>
+        <v>20</v>
+      </c>
+      <c r="F23" s="1">
+        <f>$D$23-($D$23/(COLUMNS(E5:G5))*COLUMNS(E5:F5))</f>
         <v>10</v>
       </c>
-      <c r="F12" s="18">
-        <f>E12-SUM(F6:F10)</f>
-        <v>10</v>
-      </c>
-      <c r="G12" s="49">
-        <f>F12-SUM(G6:G10)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="21">
-        <f>D12</f>
-        <v>10</v>
-      </c>
-      <c r="E13" s="22">
-        <f>$D$13-($D$13/(COLUMNS(E5:G5))*COLUMNS(E5))</f>
-        <v>6.6666666666666661</v>
-      </c>
-      <c r="F13" s="1">
-        <f>$D$13-($D$13/(COLUMNS(E5:G5))*COLUMNS(E5:F5))</f>
-        <v>3.333333333333333</v>
-      </c>
-      <c r="G13" s="2">
-        <f>$D$13-($D$13/(COLUMNS(E5:G5))*COLUMNS(E5:G5))</f>
+      <c r="G23" s="2">
+        <f>$D$23-($D$23/(COLUMNS(E5:G5))*COLUMNS(E5:G5))</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B21:C21"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>